<commit_message>
Finished Week 13 logging
</commit_message>
<xml_diff>
--- a/Base/Teams/49ers/2021 Target Depth Data.xlsx
+++ b/Base/Teams/49ers/2021 Target Depth Data.xlsx
@@ -450,22 +450,22 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>106</v>
+        <v>128</v>
       </c>
       <c r="C3">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="D3">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="E3">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -529,19 +529,19 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>84</v>
+        <v>116</v>
       </c>
       <c r="C3">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="D3">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E3">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <v>1</v>

</xml_diff>

<commit_message>
Added Week 15 simulations
</commit_message>
<xml_diff>
--- a/Base/Teams/49ers/2021 Target Depth Data.xlsx
+++ b/Base/Teams/49ers/2021 Target Depth Data.xlsx
@@ -450,16 +450,16 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>128</v>
+        <v>159</v>
       </c>
       <c r="C3">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="D3">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="E3">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -529,16 +529,16 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>116</v>
+        <v>141</v>
       </c>
       <c r="C3">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="D3">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="E3">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F3">
         <v>1</v>

</xml_diff>

<commit_message>
Logged Week 17 data and fixed Simulate_Season.py tiebreaking method
</commit_message>
<xml_diff>
--- a/Base/Teams/49ers/2021 Target Depth Data.xlsx
+++ b/Base/Teams/49ers/2021 Target Depth Data.xlsx
@@ -427,22 +427,22 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>176</v>
+        <v>191</v>
       </c>
       <c r="C2">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="D2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E2">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F2">
         <v>4</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -506,19 +506,19 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>219</v>
+        <v>248</v>
       </c>
       <c r="C2">
-        <v>149</v>
+        <v>168</v>
       </c>
       <c r="D2">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E2">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G2">
         <v>1</v>

</xml_diff>

<commit_message>
Logged 2021 divisional round, simulated season from conference round
</commit_message>
<xml_diff>
--- a/Base/Teams/49ers/2021 Target Depth Data.xlsx
+++ b/Base/Teams/49ers/2021 Target Depth Data.xlsx
@@ -450,19 +450,19 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>231</v>
+        <v>248</v>
       </c>
       <c r="C3">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="D3">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E3">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G3">
         <v>4</v>
@@ -529,16 +529,16 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>231</v>
+        <v>254</v>
       </c>
       <c r="C3">
-        <v>171</v>
+        <v>189</v>
       </c>
       <c r="D3">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E3">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F3">
         <v>2</v>

</xml_diff>

<commit_message>
Simulated ang logged 2021 conference championships
</commit_message>
<xml_diff>
--- a/Base/Teams/49ers/2021 Target Depth Data.xlsx
+++ b/Base/Teams/49ers/2021 Target Depth Data.xlsx
@@ -450,19 +450,19 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>248</v>
+        <v>273</v>
       </c>
       <c r="C3">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="D3">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E3">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G3">
         <v>4</v>
@@ -529,19 +529,19 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>254</v>
+        <v>290</v>
       </c>
       <c r="C3">
-        <v>189</v>
+        <v>216</v>
       </c>
       <c r="D3">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="E3">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G3">
         <v>3</v>

</xml_diff>